<commit_message>
Adding EndtoEnd suite and updating Excel file
</commit_message>
<xml_diff>
--- a/ecom/Resources/DataPro.xlsx
+++ b/ecom/Resources/DataPro.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC002" sheetId="1" r:id="rId1"/>
+    <sheet name="TC003" sheetId="2" r:id="rId2"/>
+    <sheet name="TC004" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>UserName</t>
   </si>
@@ -54,19 +56,70 @@
   </si>
   <si>
     <t>^%&amp;%%^</t>
+  </si>
+  <si>
+    <t>Product Id</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>MenuName</t>
+  </si>
+  <si>
+    <t>Dresses</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Expected Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -434,4 +488,159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating End to End Suite
</commit_message>
<xml_diff>
--- a/ecom/Resources/DataPro.xlsx
+++ b/ecom/Resources/DataPro.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC002" sheetId="1" r:id="rId1"/>
     <sheet name="TC003" sheetId="2" r:id="rId2"/>
     <sheet name="TC004" sheetId="3" r:id="rId3"/>
+    <sheet name="TC005" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>UserName</t>
   </si>
@@ -550,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -643,4 +644,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding break in the select color method to avoid stale element exception
</commit_message>
<xml_diff>
--- a/ecom/Resources/DataPro.xlsx
+++ b/ecom/Resources/DataPro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC002" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>UserName</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Expected Count</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -551,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding functional test case for registration email text field
</commit_message>
<xml_diff>
--- a/ecom/Resources/DataPro.xlsx
+++ b/ecom/Resources/DataPro.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\XcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\Project2MavenBranch\ecom\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TC002" sheetId="1" r:id="rId1"/>
     <sheet name="TC003" sheetId="2" r:id="rId2"/>
     <sheet name="TC004" sheetId="3" r:id="rId3"/>
     <sheet name="TC005" sheetId="4" r:id="rId4"/>
+    <sheet name="TC007" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>UserName</t>
   </si>
@@ -105,13 +106,37 @@
   </si>
   <si>
     <t>Yellow</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>mermiden@gmail.com</t>
+  </si>
+  <si>
+    <t>mermidengmail.com</t>
+  </si>
+  <si>
+    <t>mermiden@gmailcom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   </t>
+  </si>
+  <si>
+    <t>asddfgghl</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>mermiden#gmail com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +149,14 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,14 +176,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -696,4 +732,73 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4" display="mermiden@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>